<commit_message>
added clear-cart. Need to fix Add-Cart size deltas
</commit_message>
<xml_diff>
--- a/Steward Logistics.xlsx
+++ b/Steward Logistics.xlsx
@@ -197,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -205,21 +205,26 @@
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
       <color rgb="FF222222"/>
-      <name val="Open Sans"/>
+      <name val="Myriad-pro"/>
+    </font>
+    <font>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
       <color rgb="FF222222"/>
-      <name val="Open Sans"/>
+      <name val="Myriad-pro"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
       <color rgb="FF222222"/>
-      <name val="Open Sans"/>
+      <name val="Myriad-pro"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF222222"/>
+      <name val="Myriad-pro"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -246,33 +251,36 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -292,1055 +300,1091 @@
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="87.71"/>
-    <col customWidth="1" min="2" max="6" width="14.43"/>
+    <col customWidth="1" min="2" max="5" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
         <v>2.0</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
         <v>2.0</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
         <v>2.0</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
         <v>2.0</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
         <v>2.0</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
         <v>2.0</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
         <v>2.0</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
         <v>2.0</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
         <v>2.0</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
         <v>2.0</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2">
         <v>2.0</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="B48" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="B49" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="B50" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="B51" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="B52" s="2">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="B53" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="B54" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="5" t="s">
         <v>54</v>
       </c>
+      <c r="B55" s="6">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="B56" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
+      <c r="B57" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
+      <c r="B58" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="5" t="s">
         <v>58</v>
       </c>
+      <c r="B59" s="6">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="4"/>
+      <c r="A60" s="7"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="4"/>
+      <c r="A61" s="7"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="4"/>
+      <c r="A62" s="7"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="4"/>
+      <c r="A63" s="7"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="4"/>
+      <c r="A64" s="7"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="4"/>
+      <c r="A65" s="7"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="4"/>
+      <c r="A66" s="7"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="4"/>
+      <c r="A67" s="7"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="4"/>
+      <c r="A68" s="7"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="4"/>
+      <c r="A69" s="7"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="4"/>
+      <c r="A70" s="7"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="4"/>
+      <c r="A71" s="7"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="4"/>
+      <c r="A72" s="7"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="4"/>
+      <c r="A73" s="7"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="4"/>
+      <c r="A74" s="7"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="4"/>
+      <c r="A75" s="7"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="4"/>
+      <c r="A76" s="7"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="4"/>
+      <c r="A77" s="7"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="4"/>
+      <c r="A78" s="7"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="4"/>
+      <c r="A79" s="7"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="4"/>
+      <c r="A80" s="7"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="4"/>
+      <c r="A81" s="7"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="4"/>
+      <c r="A82" s="7"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="4"/>
+      <c r="A83" s="7"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="4"/>
+      <c r="A84" s="7"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="4"/>
+      <c r="A85" s="7"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="4"/>
+      <c r="A86" s="7"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="4"/>
+      <c r="A87" s="7"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="4"/>
+      <c r="A88" s="7"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="4"/>
+      <c r="A89" s="7"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="4"/>
+      <c r="A90" s="7"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="4"/>
+      <c r="A91" s="7"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="4"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="4"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="4"/>
+      <c r="A93" s="7"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="4"/>
+      <c r="A94" s="7"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="4"/>
+      <c r="A95" s="7"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="4"/>
+      <c r="A96" s="7"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="4"/>
+      <c r="A97" s="7"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="4"/>
+      <c r="A98" s="7"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="4"/>
+      <c r="A99" s="7"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="4"/>
+      <c r="A100" s="7"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="4"/>
+      <c r="A101" s="7"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="4"/>
+      <c r="A102" s="7"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="4"/>
+      <c r="A103" s="7"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="4"/>
+      <c r="A104" s="7"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="4"/>
+      <c r="A105" s="7"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="4"/>
+      <c r="A106" s="7"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="4"/>
+      <c r="A107" s="7"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="4"/>
+      <c r="A108" s="7"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="4"/>
+      <c r="A109" s="7"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="4"/>
+      <c r="A110" s="7"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="4"/>
+      <c r="A111" s="7"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="4"/>
+      <c r="A112" s="7"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="4"/>
+      <c r="A113" s="7"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="4"/>
+      <c r="A114" s="7"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="4"/>
+      <c r="A115" s="7"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="4"/>
+      <c r="A116" s="7"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="4"/>
+      <c r="A117" s="7"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="4"/>
+      <c r="A118" s="7"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="4"/>
+      <c r="A119" s="7"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="4"/>
+      <c r="A120" s="7"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="4"/>
+      <c r="A121" s="7"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="4"/>
+      <c r="A122" s="7"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="4"/>
+      <c r="A123" s="7"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="4"/>
+      <c r="A124" s="7"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="4"/>
+      <c r="A125" s="7"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="4"/>
+      <c r="A126" s="7"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="4"/>
+      <c r="A127" s="7"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="4"/>
+      <c r="A128" s="7"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="4"/>
+      <c r="A129" s="7"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="4"/>
+      <c r="A130" s="7"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="4"/>
+      <c r="A131" s="7"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="4"/>
+      <c r="A132" s="7"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="4"/>
+      <c r="A133" s="7"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="4"/>
+      <c r="A134" s="7"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="4"/>
+      <c r="A135" s="7"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="4"/>
+      <c r="A136" s="7"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="4"/>
+      <c r="A137" s="7"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="4"/>
+      <c r="A138" s="7"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="4"/>
+      <c r="A139" s="7"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="4"/>
+      <c r="A140" s="7"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="4"/>
+      <c r="A141" s="7"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="4"/>
+      <c r="A142" s="7"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="4"/>
+      <c r="A143" s="7"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="4"/>
+      <c r="A144" s="7"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="4"/>
+      <c r="A145" s="7"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="4"/>
+      <c r="A146" s="7"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="4"/>
+      <c r="A147" s="7"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="4"/>
+      <c r="A148" s="7"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="4"/>
+      <c r="A149" s="7"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="4"/>
+      <c r="A150" s="7"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="4"/>
+      <c r="A151" s="7"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="4"/>
+      <c r="A152" s="7"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="4"/>
+      <c r="A153" s="7"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="4"/>
+      <c r="A154" s="7"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="4"/>
+      <c r="A155" s="7"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="4"/>
+      <c r="A156" s="7"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="4"/>
+      <c r="A157" s="7"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="4"/>
+      <c r="A158" s="7"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="4"/>
+      <c r="A159" s="7"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="4"/>
+      <c r="A160" s="7"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="4"/>
+      <c r="A161" s="7"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="4"/>
+      <c r="A162" s="7"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="4"/>
+      <c r="A163" s="7"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="4"/>
+      <c r="A164" s="7"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="4"/>
+      <c r="A165" s="7"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="4"/>
+      <c r="A166" s="7"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="4"/>
+      <c r="A167" s="7"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="4"/>
+      <c r="A168" s="7"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="4"/>
+      <c r="A169" s="7"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="4"/>
+      <c r="A170" s="7"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="4"/>
+      <c r="A171" s="7"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="4"/>
+      <c r="A172" s="7"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="4"/>
+      <c r="A173" s="7"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="4"/>
+      <c r="A174" s="7"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="4"/>
+      <c r="A175" s="7"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="4"/>
+      <c r="A176" s="7"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="4"/>
+      <c r="A177" s="7"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="4"/>
+      <c r="A178" s="7"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="4"/>
+      <c r="A179" s="7"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="4"/>
+      <c r="A180" s="7"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="A181" s="4"/>
+      <c r="A181" s="7"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="A182" s="4"/>
+      <c r="A182" s="7"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="4"/>
+      <c r="A183" s="7"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="4"/>
+      <c r="A184" s="7"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="4"/>
+      <c r="A185" s="7"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="4"/>
+      <c r="A186" s="7"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="A187" s="4"/>
+      <c r="A187" s="7"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="A188" s="4"/>
+      <c r="A188" s="7"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="A189" s="4"/>
+      <c r="A189" s="7"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="A190" s="4"/>
+      <c r="A190" s="7"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="A191" s="4"/>
+      <c r="A191" s="7"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="A192" s="4"/>
+      <c r="A192" s="7"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="4"/>
+      <c r="A193" s="7"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="4"/>
+      <c r="A194" s="7"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="4"/>
+      <c r="A195" s="7"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="4"/>
+      <c r="A196" s="7"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="4"/>
+      <c r="A197" s="7"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="4"/>
+      <c r="A198" s="7"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="4"/>
+      <c r="A199" s="7"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="4"/>
+      <c r="A200" s="7"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="4"/>
+      <c r="A201" s="7"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="4"/>
+      <c r="A202" s="7"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="4"/>
+      <c r="A203" s="7"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="4"/>
+      <c r="A204" s="7"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="4"/>
+      <c r="A205" s="7"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="4"/>
+      <c r="A206" s="7"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="4"/>
+      <c r="A207" s="7"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="4"/>
+      <c r="A208" s="7"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="4"/>
+      <c r="A209" s="7"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="4"/>
+      <c r="A210" s="7"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="4"/>
+      <c r="A211" s="7"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="4"/>
+      <c r="A212" s="7"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="4"/>
+      <c r="A213" s="7"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="4"/>
+      <c r="A214" s="7"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="4"/>
+      <c r="A215" s="7"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="4"/>
+      <c r="A216" s="7"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="4"/>
+      <c r="A217" s="7"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="4"/>
+      <c r="A218" s="7"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="A219" s="4"/>
+      <c r="A219" s="7"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="4"/>
+      <c r="A220" s="7"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="4"/>
+      <c r="A221" s="7"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="4"/>
+      <c r="A222" s="7"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="4"/>
+      <c r="A223" s="7"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="4"/>
+      <c r="A224" s="7"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="4"/>
+      <c r="A225" s="7"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="4"/>
+      <c r="A226" s="7"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="4"/>
+      <c r="A227" s="7"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="A228" s="4"/>
+      <c r="A228" s="7"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="A229" s="4"/>
+      <c r="A229" s="7"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="A230" s="4"/>
+      <c r="A230" s="7"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="A231" s="4"/>
+      <c r="A231" s="7"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="4"/>
+      <c r="A232" s="7"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="A233" s="4"/>
+      <c r="A233" s="7"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="A234" s="4"/>
+      <c r="A234" s="7"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="A235" s="4"/>
+      <c r="A235" s="7"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="A236" s="4"/>
+      <c r="A236" s="7"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="4"/>
+      <c r="A237" s="7"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="A238" s="4"/>
+      <c r="A238" s="7"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="A239" s="4"/>
+      <c r="A239" s="7"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="A240" s="4"/>
+      <c r="A240" s="7"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="A241" s="4"/>
+      <c r="A241" s="7"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="A242" s="4"/>
+      <c r="A242" s="7"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="A243" s="4"/>
+      <c r="A243" s="7"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="A244" s="4"/>
+      <c r="A244" s="7"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="A245" s="4"/>
+      <c r="A245" s="7"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="A246" s="4"/>
+      <c r="A246" s="7"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="A247" s="4"/>
+      <c r="A247" s="7"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="A248" s="4"/>
+      <c r="A248" s="7"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="A249" s="4"/>
+      <c r="A249" s="7"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="A250" s="4"/>
+      <c r="A250" s="7"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="A251" s="4"/>
+      <c r="A251" s="7"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="A252" s="4"/>
+      <c r="A252" s="7"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="A253" s="4"/>
+      <c r="A253" s="7"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="A254" s="4"/>
+      <c r="A254" s="7"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="A255" s="4"/>
+      <c r="A255" s="7"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="A256" s="4"/>
+      <c r="A256" s="7"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="A257" s="4"/>
+      <c r="A257" s="7"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="A258" s="4"/>
+      <c r="A258" s="7"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="A259" s="4"/>
+      <c r="A259" s="7"/>
     </row>
     <row r="260" ht="15.75" customHeight="1"/>
     <row r="261" ht="15.75" customHeight="1"/>

</xml_diff>